<commit_message>
Updated layout for agile artifacts before release planning
</commit_message>
<xml_diff>
--- a/agile_artifacts/SprintBackLog.xlsx
+++ b/agile_artifacts/SprintBackLog.xlsx
@@ -8,12 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\school_code\CST-247-Project\agile_artifacts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B85342BC-E777-434F-8775-E046A7978719}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD38380B-4002-4D35-99BD-7BCE0F6F3734}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="28800" windowHeight="11385" xr2:uid="{8866F3F1-5DE4-42AB-826D-82D67BF29B9B}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="26355" windowHeight="15600" xr2:uid="{8866F3F1-5DE4-42AB-826D-82D67BF29B9B}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="MIlestone 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Milestone 2" sheetId="2" r:id="rId2"/>
+    <sheet name="Milestone 3" sheetId="3" r:id="rId3"/>
+    <sheet name="Milestone 4" sheetId="4" r:id="rId4"/>
+    <sheet name="Milestone 5" sheetId="5" r:id="rId5"/>
+    <sheet name="MIlestone 6" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,9 +38,191 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="19">
+  <si>
+    <t>Task ID</t>
+  </si>
+  <si>
+    <t>Assigned</t>
+  </si>
+  <si>
+    <t>Task</t>
+  </si>
+  <si>
+    <t>Requirement</t>
+  </si>
+  <si>
+    <t>Sizing</t>
+  </si>
+  <si>
+    <t>Actual</t>
+  </si>
+  <si>
+    <t>Code Review</t>
+  </si>
+  <si>
+    <t>QA</t>
+  </si>
+  <si>
+    <t>Tester Assigned</t>
+  </si>
+  <si>
+    <t>SP1</t>
+  </si>
+  <si>
+    <t>Release Planning</t>
+  </si>
+  <si>
+    <t>Richard &amp; Shawn</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Goal: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Plan the release of the Minesweeper Game Service</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Goal: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Login and Registration completed</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Goal: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Initial Game Board module adapted from previous class</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Goal: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Gameboard Module to be finished</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Goal: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Ability to save/Restore game progress as well as REST API for fetching this data</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Goal: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Precentation of final project, along with completed game service.</t>
+    </r>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -43,16 +230,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -60,12 +261,36 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -380,14 +605,432 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BF1D55D-F0C0-4D4A-BED7-2F05F7B7D26B}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="52.85546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="7"/>
+    <col min="7" max="7" width="12.42578125" customWidth="1"/>
+    <col min="9" max="9" width="15.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+    </row>
+    <row r="2" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="7">
+        <v>2</v>
+      </c>
+      <c r="G3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:I1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBB8A355-FAFD-415E-B394-187D4F8A7B0C}">
+  <dimension ref="A1:I2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="52.85546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="7"/>
+    <col min="7" max="7" width="12.42578125" customWidth="1"/>
+    <col min="9" max="9" width="15.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+    </row>
+    <row r="2" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:I1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E296FE81-BE99-43CC-8FB4-CB8D27E2DC42}">
+  <dimension ref="A1:I2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="52.85546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="7"/>
+    <col min="7" max="7" width="12.42578125" customWidth="1"/>
+    <col min="9" max="9" width="15.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+    </row>
+    <row r="2" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:I1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCDCFAD7-7229-440F-B3DD-D6BC9D1B4560}">
+  <dimension ref="A1:I2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="52.85546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="7"/>
+    <col min="7" max="7" width="12.42578125" customWidth="1"/>
+    <col min="9" max="9" width="15.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+    </row>
+    <row r="2" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:I1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17959530-2D57-4878-A9F5-A99D202A70AF}">
+  <dimension ref="A1:I2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="52.85546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="7"/>
+    <col min="7" max="7" width="12.42578125" customWidth="1"/>
+    <col min="9" max="9" width="15.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+    </row>
+    <row r="2" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:I1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C05895A4-8B70-4CB9-A697-93FA09E903E1}">
+  <dimension ref="A1:I2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="52.85546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="7"/>
+    <col min="7" max="7" width="12.42578125" customWidth="1"/>
+    <col min="9" max="9" width="15.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+    </row>
+    <row r="2" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:I1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>